<commit_message>
Changes Related to HomeTiles.
</commit_message>
<xml_diff>
--- a/managementcmdfiles/choice.xlsx
+++ b/managementcmdfiles/choice.xlsx
@@ -1474,7 +1474,7 @@
     <t xml:space="preserve">relational operator</t>
   </si>
   <si>
-    <t xml:space="preserve">is </t>
+    <t xml:space="preserve">is</t>
   </si>
   <si>
     <t xml:space="preserve">is_not</t>
@@ -1728,9 +1728,9 @@
   <dimension ref="A1:F445"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B315" activeCellId="0" sqref="B315"/>
+      <selection pane="bottomLeft" activeCell="D398" activeCellId="0" sqref="D398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>